<commit_message>
Fix ten tu dong them ncc + ngay nhap
</commit_message>
<xml_diff>
--- a/initalBook.xlsx
+++ b/initalBook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\KTPM-BookShop\KTPM-BookShop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\KTPM-BookShop1\KTPM-BookShop\KTPM-BookShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208B966C-F970-486C-BC48-C76792E7375B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818AF1F6-FA21-40D9-8FB0-DB78E638D7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Mã nhà cung cấp</t>
   </si>
@@ -31,70 +31,31 @@
     <t>số lượng</t>
   </si>
   <si>
-    <t>Giá nhập</t>
-  </si>
-  <si>
-    <t>Cho tôi một vé đi tuổi thơ</t>
-  </si>
-  <si>
     <t>Số thứ tự</t>
   </si>
   <si>
-    <t>Conan</t>
+    <t>Phần trăm lãi suất</t>
   </si>
   <si>
-    <t>Năm mươi Sắc thái</t>
+    <t>Giá bán</t>
   </si>
   <si>
-    <t>Chiến Thắng Con Quỷ Trong Bạn</t>
+    <t>Conan 1</t>
   </si>
   <si>
-    <t>Đất Rừng Phương Nam</t>
+    <t>Năm mươi Sắc thái 1</t>
   </si>
   <si>
-    <t>Harry Potter Và Hòn Đá Phù Thuỷ</t>
+    <t>Cho tôi một vé đi tuổi thơ 2</t>
   </si>
   <si>
-    <t>Đắc Nhân Tâm</t>
+    <t>Chiến Thắng Con Quỷ Trong Bạn 3</t>
   </si>
   <si>
-    <t>Harry Potter Và Phòng Chứa Bí Mật</t>
+    <t>Đất Rừng Phương Nam 4</t>
   </si>
   <si>
-    <t>Nguyên Tắc Vàng Của Napoleon Hill</t>
-  </si>
-  <si>
-    <t>Nghĩ giàu làm giàu</t>
-  </si>
-  <si>
-    <t>Tết ở làng địa ngục</t>
-  </si>
-  <si>
-    <t>Thiền Sư Và Em Bé 5 Tuổi</t>
-  </si>
-  <si>
-    <t>Trần Văn Ơn</t>
-  </si>
-  <si>
-    <t>Thuật Thao Túng  Góc Tối Ẩn Sau Mỗi Câu Nói</t>
-  </si>
-  <si>
-    <t>Đám trẻ ở đại dương đen</t>
-  </si>
-  <si>
-    <t>Tôi thấy hoa vàng trên cỏ xanh</t>
-  </si>
-  <si>
-    <t>Sức mạnh của ngôn từ</t>
-  </si>
-  <si>
-    <t>Life Skills</t>
-  </si>
-  <si>
-    <t>Sĩ số lớp vắng không</t>
-  </si>
-  <si>
-    <t>Cây cam ngọt của tôi</t>
+    <t>Harry Potter Và Hòn Đá Phù Thuỷ 4</t>
   </si>
 </sst>
 </file>
@@ -370,7 +331,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -390,10 +351,16 @@
       <c r="B1" s="1">
         <v>3</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -402,7 +369,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -438,7 +405,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -452,7 +419,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -466,7 +433,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -480,7 +447,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -490,200 +457,81 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>50000</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>100000</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="3">
-        <v>1</v>
-      </c>
-      <c r="D11" s="3">
-        <v>80000</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <v>60000</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>82000</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>80000</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3">
-        <v>15000</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>95000</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>15000</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>115000</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
-        <v>17</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>10000</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>198000</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>19</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="3">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>70000</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
-        <v>20</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
-      </c>
-      <c r="D22">
-        <v>85000</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix xoa san pham > 7 ngay
</commit_message>
<xml_diff>
--- a/initalBook.xlsx
+++ b/initalBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\KTPM-BookShop1\KTPM-BookShop\KTPM-BookShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818AF1F6-FA21-40D9-8FB0-DB78E638D7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913866FF-6AB8-4033-A729-3FDBEE19E84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -331,7 +331,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="E14" sqref="E14:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix loi ko ton tai maKhuyenMai (trang ban sach)
</commit_message>
<xml_diff>
--- a/initalBook.xlsx
+++ b/initalBook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\KTPM-BookShop1\KTPM-BookShop\KTPM-BookShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913866FF-6AB8-4033-A729-3FDBEE19E84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD6C8E-DD7E-4EF8-B273-AC9DC28E71BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,22 +40,22 @@
     <t>Giá bán</t>
   </si>
   <si>
-    <t>Conan 1</t>
+    <t>Conan</t>
   </si>
   <si>
-    <t>Năm mươi Sắc thái 1</t>
+    <t>Cho tôi một vé đi tuổi thơ</t>
   </si>
   <si>
-    <t>Cho tôi một vé đi tuổi thơ 2</t>
+    <t>Năm mươi Sắc thái</t>
   </si>
   <si>
-    <t>Chiến Thắng Con Quỷ Trong Bạn 3</t>
+    <t>Đất Rừng Phương Nam</t>
   </si>
   <si>
-    <t>Đất Rừng Phương Nam 4</t>
+    <t>Harry Potter Và Hòn Đá Phù Thuỷ</t>
   </si>
   <si>
-    <t>Harry Potter Và Hòn Đá Phù Thuỷ 4</t>
+    <t>Chiến Thắng Con Quỷ Trong Bạn</t>
   </si>
 </sst>
 </file>
@@ -331,7 +331,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:M15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -380,7 +380,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3">
         <v>80000</v>
@@ -391,10 +391,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>115000</v>
@@ -405,10 +405,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D5" s="3">
         <v>80000</v>
@@ -419,10 +419,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3">
         <v>110000</v>
@@ -433,10 +433,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3">
         <v>65000</v>
@@ -447,10 +447,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D8" s="3">
         <v>115000</v>

</xml_diff>

<commit_message>
Fix ban hang do khuyen mai + fix lai vu cap nhat gia
</commit_message>
<xml_diff>
--- a/initalBook.xlsx
+++ b/initalBook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\KTPM-BookShop1\KTPM-BookShop\KTPM-BookShop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\KTPM-BookShop1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD6C8E-DD7E-4EF8-B273-AC9DC28E71BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522D2C27-B343-4FE7-BE1F-3F7170721C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Mã nhà cung cấp</t>
   </si>
@@ -31,22 +31,19 @@
     <t>số lượng</t>
   </si>
   <si>
-    <t>Số thứ tự</t>
+    <t>Cho tôi một vé đi tuổi thơ</t>
   </si>
   <si>
-    <t>Phần trăm lãi suất</t>
-  </si>
-  <si>
-    <t>Giá bán</t>
+    <t>Số thứ tự</t>
   </si>
   <si>
     <t>Conan</t>
   </si>
   <si>
-    <t>Cho tôi một vé đi tuổi thơ</t>
+    <t>Năm mươi Sắc thái</t>
   </si>
   <si>
-    <t>Năm mươi Sắc thái</t>
+    <t>Chiến Thắng Con Quỷ Trong Bạn</t>
   </si>
   <si>
     <t>Đất Rừng Phương Nam</t>
@@ -55,7 +52,19 @@
     <t>Harry Potter Và Hòn Đá Phù Thuỷ</t>
   </si>
   <si>
-    <t>Chiến Thắng Con Quỷ Trong Bạn</t>
+    <t>Đắc Nhân Tâm</t>
+  </si>
+  <si>
+    <t>Harry Potter Và Phòng Chứa Bí Mật</t>
+  </si>
+  <si>
+    <t>Nguyên Tắc Vàng Của Napoleon Hill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giá bìa </t>
+  </si>
+  <si>
+    <t>Phần trăm lợi nhuận</t>
   </si>
 </sst>
 </file>
@@ -331,7 +340,7 @@
   <dimension ref="A1:D999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A12" sqref="A12:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -352,7 +361,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D1">
         <v>40</v>
@@ -360,7 +369,7 @@
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -369,7 +378,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -377,7 +386,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3">
         <v>50</v>
@@ -391,7 +400,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3">
         <v>50</v>
@@ -405,7 +414,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3">
         <v>50</v>
@@ -419,7 +428,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3">
         <v>50</v>
@@ -433,7 +442,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
         <v>50</v>
@@ -447,7 +456,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="3">
         <v>50</v>
@@ -457,22 +466,46 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="3">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3">
+        <v>50000</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3">
+        <v>100000</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="3">
+        <v>50</v>
+      </c>
+      <c r="D11" s="3">
+        <v>80000</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>

</xml_diff>